<commit_message>
edit and del excel
</commit_message>
<xml_diff>
--- a/db/excel/media.xlsx
+++ b/db/excel/media.xlsx
@@ -216,9 +216,6 @@
     <t>Các hàm API của hệ thống</t>
   </si>
   <si>
-    <t>Trả về các chức năng cần phân quyền (has_granted), để thực hiện gán quyền cho nhóm quyền hoặc user</t>
-  </si>
-  <si>
     <t>Lấy danh sách nhóm quyền</t>
   </si>
   <si>
@@ -289,6 +286,9 @@
   </si>
   <si>
     <t>/test</t>
+  </si>
+  <si>
+    <t>Trả về các chức năng</t>
   </si>
 </sst>
 </file>
@@ -2704,7 +2704,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2715,7 +2715,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2726,7 +2726,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2737,7 +2737,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2748,7 +2748,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2764,7 +2764,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2777,7 +2777,9 @@
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="30.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" customWidth="1"/>
     <col min="14" max="14" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2786,28 +2788,28 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="22" t="s">
         <v>36</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>37</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>17</v>
@@ -2819,10 +2821,10 @@
         <v>0</v>
       </c>
       <c r="M1" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="23" t="s">
         <v>38</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2833,13 +2835,13 @@
         <v>24</v>
       </c>
       <c r="C2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="19" t="s">
-        <v>50</v>
-      </c>
       <c r="E2" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F2" s="19">
         <v>1</v>
@@ -2853,13 +2855,13 @@
         <v>25</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="L2" s="19">
         <v>1</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N2" s="21"/>
     </row>
@@ -2868,16 +2870,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>50</v>
-      </c>
       <c r="E3" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" s="19">
         <v>1</v>
@@ -2888,16 +2890,16 @@
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="20" t="s">
         <v>27</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>28</v>
       </c>
       <c r="L3" s="19">
         <v>1</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N3" s="21"/>
     </row>

</xml_diff>